<commit_message>
refining categories and fixing coloring bug
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/voidant/Desktop/calculations/Orostara-Dictionary/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4980BD6E-F042-2940-9C11-BC3CF71C6510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C49E79C-DFA7-034E-9F75-C3AB2D5ACB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10620" yWindow="500" windowWidth="22980" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6053" uniqueCount="3911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6054" uniqueCount="3911">
   <si>
     <t>Notes</t>
   </si>
@@ -12700,8 +12700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O912"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="K150" sqref="K150"/>
+    <sheetView tabSelected="1" topLeftCell="A551" zoomScale="118" workbookViewId="0">
+      <selection activeCell="J569" sqref="J569"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12959,6 +12959,9 @@
       <c r="J10" t="s">
         <v>3903</v>
       </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
       <c r="L10" t="s">
         <v>10</v>
       </c>
@@ -13640,9 +13643,6 @@
       <c r="G38" t="s">
         <v>1763</v>
       </c>
-      <c r="K38">
-        <v>5</v>
-      </c>
       <c r="L38" t="s">
         <v>2843</v>
       </c>
@@ -13666,6 +13666,9 @@
       <c r="I39" t="s">
         <v>93</v>
       </c>
+      <c r="K39">
+        <v>5</v>
+      </c>
       <c r="L39" t="s">
         <v>45</v>
       </c>
@@ -15187,6 +15190,9 @@
       <c r="F106" t="s">
         <v>187</v>
       </c>
+      <c r="K106">
+        <v>6</v>
+      </c>
       <c r="L106" t="s">
         <v>107</v>
       </c>
@@ -15317,6 +15323,9 @@
       <c r="J111" t="s">
         <v>3903</v>
       </c>
+      <c r="K111">
+        <v>5</v>
+      </c>
       <c r="L111" t="s">
         <v>36</v>
       </c>
@@ -15452,9 +15461,6 @@
       </c>
       <c r="J118" t="s">
         <v>3900</v>
-      </c>
-      <c r="K118">
-        <v>22</v>
       </c>
       <c r="L118" t="s">
         <v>2843</v>
@@ -17367,6 +17373,9 @@
       <c r="J210" t="s">
         <v>3903</v>
       </c>
+      <c r="K210">
+        <v>3</v>
+      </c>
       <c r="L210" t="s">
         <v>22</v>
       </c>
@@ -19582,6 +19591,12 @@
       <c r="G307" t="s">
         <v>1882</v>
       </c>
+      <c r="I307" t="s">
+        <v>3885</v>
+      </c>
+      <c r="K307">
+        <v>2</v>
+      </c>
       <c r="L307" t="s">
         <v>177</v>
       </c>
@@ -23624,6 +23639,9 @@
       <c r="J493" t="s">
         <v>3903</v>
       </c>
+      <c r="K493">
+        <v>6</v>
+      </c>
       <c r="L493" t="s">
         <v>36</v>
       </c>
@@ -24488,6 +24506,9 @@
       <c r="J532" t="s">
         <v>3903</v>
       </c>
+      <c r="K532">
+        <v>8</v>
+      </c>
       <c r="L532" t="s">
         <v>70</v>
       </c>
@@ -24980,6 +25001,9 @@
       <c r="J553" t="s">
         <v>3903</v>
       </c>
+      <c r="K553">
+        <v>10</v>
+      </c>
       <c r="L553" t="s">
         <v>70</v>
       </c>
@@ -25438,6 +25462,9 @@
       <c r="I574" t="s">
         <v>3881</v>
       </c>
+      <c r="K574">
+        <v>1</v>
+      </c>
       <c r="L574" t="s">
         <v>70</v>
       </c>
@@ -25664,6 +25691,9 @@
       <c r="I585" t="s">
         <v>3885</v>
       </c>
+      <c r="K585">
+        <v>0</v>
+      </c>
       <c r="L585" t="s">
         <v>64</v>
       </c>
@@ -26431,6 +26461,9 @@
       <c r="I618" t="s">
         <v>3885</v>
       </c>
+      <c r="K618">
+        <v>4</v>
+      </c>
       <c r="L618" t="s">
         <v>45</v>
       </c>
@@ -26454,6 +26487,9 @@
       <c r="I619" t="s">
         <v>93</v>
       </c>
+      <c r="K619">
+        <v>0</v>
+      </c>
       <c r="L619" t="s">
         <v>10</v>
       </c>
@@ -26918,6 +26954,9 @@
       <c r="I641" t="s">
         <v>3885</v>
       </c>
+      <c r="K641">
+        <v>5</v>
+      </c>
       <c r="L641" t="s">
         <v>22</v>
       </c>
@@ -28391,6 +28430,9 @@
       <c r="J704" t="s">
         <v>3903</v>
       </c>
+      <c r="K704">
+        <v>4</v>
+      </c>
       <c r="L704" t="s">
         <v>59</v>
       </c>
@@ -29642,6 +29684,9 @@
       <c r="I758" t="s">
         <v>3885</v>
       </c>
+      <c r="K758">
+        <v>3</v>
+      </c>
       <c r="L758" t="s">
         <v>107</v>
       </c>
@@ -29760,6 +29805,9 @@
       <c r="J763" t="s">
         <v>3903</v>
       </c>
+      <c r="K763">
+        <v>2</v>
+      </c>
       <c r="L763" t="s">
         <v>66</v>
       </c>
@@ -30832,6 +30880,9 @@
       <c r="I811" t="s">
         <v>1099</v>
       </c>
+      <c r="K811">
+        <v>0</v>
+      </c>
       <c r="L811" t="s">
         <v>22</v>
       </c>
@@ -31759,6 +31810,9 @@
       <c r="J853" t="s">
         <v>3903</v>
       </c>
+      <c r="K853">
+        <v>7</v>
+      </c>
       <c r="L853" t="s">
         <v>175</v>
       </c>
@@ -32144,6 +32198,9 @@
       </c>
       <c r="J871" t="s">
         <v>3903</v>
+      </c>
+      <c r="K871">
+        <v>1</v>
       </c>
       <c r="L871" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
tweaking body order again
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/voidant/Desktop/calculations/Orostara-Dictionary/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AF12C0-1894-9F45-9706-84C2D1E859C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E164D10-9670-D548-A050-AAF4C89CA87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5860" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6109" uniqueCount="3942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6110" uniqueCount="3942">
   <si>
     <t>Orostara</t>
   </si>
@@ -12732,8 +12732,8 @@
   <dimension ref="A1:O920"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G930" sqref="G930"/>
+      <pane ySplit="1" topLeftCell="A489" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K510" sqref="K510"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14901,7 +14901,7 @@
         <v>397</v>
       </c>
       <c r="K93">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="L93" t="s">
         <v>110</v>
@@ -21263,7 +21263,7 @@
         <v>397</v>
       </c>
       <c r="K382">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L382" t="s">
         <v>0</v>
@@ -21610,6 +21610,9 @@
       <c r="D397" t="s">
         <v>3938</v>
       </c>
+      <c r="I397" t="s">
+        <v>397</v>
+      </c>
       <c r="K397">
         <v>39</v>
       </c>
@@ -23990,6 +23993,9 @@
       <c r="I507" t="s">
         <v>397</v>
       </c>
+      <c r="K507">
+        <v>31</v>
+      </c>
       <c r="L507" t="s">
         <v>0</v>
       </c>
@@ -32437,7 +32443,7 @@
         <v>397</v>
       </c>
       <c r="K878">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L878" t="s">
         <v>576</v>
@@ -32495,7 +32501,7 @@
         <v>397</v>
       </c>
       <c r="K880">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L880" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
fixed notes formatting bug and allow for more than one root word/lang
adding 'hush' word comes loosely from a couple languages so it can now list them and their words separated by /. Also notes overflowing because of incorrect formatting stuff so I fixed that
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/voidant/Desktop/calculations/Orostara-Dictionary/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F0083E-6639-6940-9032-677D5FADE4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EEB9E5-0927-0D4E-A829-7E692DA53584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="500" windowWidth="21240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14388,7 +14388,7 @@
     <t>噓/चुप/shush/اشش</t>
   </si>
   <si>
-    <t>the x sound can be extended and the -u ending is optional in in speech; 'shhh' is said the same in English and Orostara and can also be written as 'x~~'; actually pronouncing it 'xu' is more like 'hush' or 'shush'</t>
+    <t>the x sound can be extended and the -u ending is optiona in speech; 'shhh' is said the same in English and Orostara and can also be written as 'x~~'; actually pronouncing it 'xu' is more like 'hush' or 'shush'</t>
   </si>
 </sst>
 </file>
@@ -14951,7 +14951,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -14966,7 +14966,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -15367,9 +15366,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P970"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A947" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A923" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J966" sqref="J966"/>
+      <selection pane="topRight" activeCell="I944" sqref="I944"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38858,7 +38857,7 @@
       <c r="L969" t="s">
         <v>3724</v>
       </c>
-      <c r="M969" s="14" t="s">
+      <c r="M969" t="s">
         <v>1222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing bug and dict updates
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -14902,7 +14902,7 @@
     <t xml:space="preserve">meaning changed a lot since inception; dialect dependent; here it just means anything sexual down there that’s not your dick/clit</t>
   </si>
   <si>
-    <t xml:space="preserve">vulva/scrotum/labia/taint</t>
+    <t xml:space="preserve">vulva/scrotum/labia/taint/genital</t>
   </si>
   <si>
     <t xml:space="preserve">योनी</t>
@@ -16085,10 +16085,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A965" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B965" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A965" activeCellId="0" sqref="A965"/>
-      <selection pane="topRight" activeCell="C984" activeCellId="0" sqref="C984"/>
+      <selection pane="topRight" activeCell="F976" activeCellId="0" sqref="F976"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.5"/>

</xml_diff>

<commit_message>
dict updates and all the vocab for flashcards
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7792" uniqueCount="5085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7785" uniqueCount="5080">
   <si>
     <t xml:space="preserve">Orostara</t>
   </si>
@@ -14214,21 +14214,6 @@
   </si>
   <si>
     <t xml:space="preserve">/t͡ʃʊn.nɑː/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xunar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gravity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">重力</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zhònglì</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/ʈ͡ʂʊŋ⁵¹⁻⁵³ li⁵¹/</t>
   </si>
   <si>
     <t xml:space="preserve">Xunkuamur</t>
@@ -15892,8 +15877,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P1044" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:P1044"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P1043" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:P1043"/>
   <tableColumns count="16">
     <tableColumn id="1" name="Orostara"/>
     <tableColumn id="2" name="Type"/>
@@ -15922,13 +15907,13 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B33" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
-      <selection pane="topRight" activeCell="J67" activeCellId="0" sqref="J67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A932" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B932" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A932" activeCellId="0" sqref="A932"/>
+      <selection pane="topRight" activeCell="B953" activeCellId="0" sqref="B953"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.62109375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.62890625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.5"/>
@@ -39913,18 +39898,24 @@
         <v>4678</v>
       </c>
       <c r="B953" s="0" t="s">
-        <v>23</v>
+        <v>58</v>
+      </c>
+      <c r="C953" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="D953" s="0" t="s">
         <v>4679</v>
       </c>
+      <c r="I953" s="0" t="s">
+        <v>61</v>
+      </c>
       <c r="L953" s="0" t="s">
         <v>40</v>
       </c>
       <c r="M953" s="9" t="s">
         <v>4680</v>
       </c>
-      <c r="N953" s="11" t="s">
+      <c r="N953" s="0" t="s">
         <v>4681</v>
       </c>
       <c r="O953" s="0" t="s">
@@ -39936,16 +39927,13 @@
         <v>4683</v>
       </c>
       <c r="B954" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C954" s="0" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="D954" s="0" t="s">
         <v>4684</v>
       </c>
-      <c r="I954" s="0" t="s">
-        <v>61</v>
+      <c r="E954" s="0" t="s">
+        <v>359</v>
       </c>
       <c r="L954" s="0" t="s">
         <v>40</v>
@@ -39970,46 +39958,52 @@
       <c r="D955" s="0" t="s">
         <v>4689</v>
       </c>
-      <c r="E955" s="0" t="s">
-        <v>359</v>
+      <c r="F955" s="0" t="s">
+        <v>4690</v>
+      </c>
+      <c r="G955" s="0" t="s">
+        <v>4691</v>
+      </c>
+      <c r="H955" s="0" t="s">
+        <v>4692</v>
+      </c>
+      <c r="I955" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J955" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="L955" s="0" t="s">
         <v>40</v>
       </c>
       <c r="M955" s="9" t="s">
-        <v>4690</v>
+        <v>4693</v>
       </c>
       <c r="N955" s="0" t="s">
-        <v>4691</v>
+        <v>4694</v>
       </c>
       <c r="O955" s="0" t="s">
-        <v>4692</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A956" s="0" t="s">
-        <v>4693</v>
+        <v>4696</v>
       </c>
       <c r="B956" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D956" s="0" t="s">
-        <v>4694</v>
-      </c>
-      <c r="F956" s="0" t="s">
-        <v>4695</v>
-      </c>
-      <c r="G956" s="0" t="s">
-        <v>4696</v>
-      </c>
-      <c r="H956" s="0" t="s">
+      <c r="E956" s="0" t="s">
         <v>4697</v>
       </c>
       <c r="I956" s="0" t="s">
-        <v>26</v>
+        <v>342</v>
       </c>
       <c r="J956" s="0" t="s">
-        <v>19</v>
+        <v>307</v>
+      </c>
+      <c r="K956" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="L956" s="0" t="s">
         <v>40</v>
@@ -40031,72 +40025,63 @@
       <c r="B957" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E957" s="0" t="s">
+      <c r="D957" s="0" t="s">
         <v>4702</v>
       </c>
+      <c r="H957" s="0" t="s">
+        <v>4703</v>
+      </c>
       <c r="I957" s="0" t="s">
-        <v>342</v>
+        <v>26</v>
       </c>
       <c r="J957" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="K957" s="0" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="L957" s="0" t="s">
         <v>40</v>
       </c>
       <c r="M957" s="9" t="s">
-        <v>4703</v>
+        <v>4704</v>
       </c>
       <c r="N957" s="0" t="s">
-        <v>4704</v>
+        <v>4705</v>
       </c>
       <c r="O957" s="0" t="s">
-        <v>4705</v>
+        <v>4706</v>
       </c>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A958" s="0" t="s">
-        <v>4706</v>
+        <v>4707</v>
       </c>
       <c r="B958" s="0" t="s">
-        <v>23</v>
+        <v>596</v>
+      </c>
+      <c r="C958" s="0" t="s">
+        <v>4326</v>
       </c>
       <c r="D958" s="0" t="s">
-        <v>4707</v>
-      </c>
-      <c r="H958" s="0" t="s">
         <v>4708</v>
       </c>
-      <c r="I958" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J958" s="0" t="s">
-        <v>19</v>
+      <c r="F958" s="0" t="s">
+        <v>4709</v>
       </c>
       <c r="L958" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="M958" s="9" t="s">
-        <v>4709</v>
-      </c>
-      <c r="N958" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M958" s="0" t="s">
         <v>4710</v>
-      </c>
-      <c r="O958" s="0" t="s">
-        <v>4711</v>
       </c>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A959" s="0" t="s">
+        <v>4711</v>
+      </c>
+      <c r="B959" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C959" s="0" t="s">
         <v>4712</v>
-      </c>
-      <c r="B959" s="0" t="s">
-        <v>596</v>
-      </c>
-      <c r="C959" s="0" t="s">
-        <v>4326</v>
       </c>
       <c r="D959" s="0" t="s">
         <v>4713</v>
@@ -40105,76 +40090,76 @@
         <v>4714</v>
       </c>
       <c r="L959" s="0" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="M959" s="0" t="s">
         <v>4715</v>
       </c>
+      <c r="N959" s="0" t="s">
+        <v>4711</v>
+      </c>
+      <c r="O959" s="0" t="s">
+        <v>4716</v>
+      </c>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A960" s="0" t="s">
-        <v>4716</v>
-      </c>
-      <c r="B960" s="0" t="s">
-        <v>23</v>
+        <v>4717</v>
       </c>
       <c r="C960" s="0" t="s">
-        <v>4717</v>
-      </c>
-      <c r="D960" s="0" t="s">
         <v>4718</v>
       </c>
-      <c r="F960" s="0" t="s">
+      <c r="G960" s="0" t="s">
         <v>4719</v>
       </c>
       <c r="L960" s="0" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="M960" s="0" t="s">
         <v>4720</v>
       </c>
-      <c r="N960" s="0" t="s">
-        <v>4716</v>
-      </c>
-      <c r="O960" s="0" t="s">
-        <v>4721</v>
-      </c>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A961" s="0" t="s">
+        <v>4721</v>
+      </c>
+      <c r="B961" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C961" s="0" t="s">
         <v>4722</v>
       </c>
-      <c r="C961" s="0" t="s">
+      <c r="D961" s="0" t="s">
+        <v>3920</v>
+      </c>
+      <c r="I961" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="K961" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L961" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M961" s="0" t="s">
         <v>4723</v>
       </c>
-      <c r="G961" s="0" t="s">
+      <c r="N961" s="0" t="s">
         <v>4724</v>
-      </c>
-      <c r="L961" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M961" s="0" t="s">
-        <v>4725</v>
       </c>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A962" s="0" t="s">
+        <v>4725</v>
+      </c>
+      <c r="E962" s="0" t="s">
         <v>4726</v>
       </c>
-      <c r="B962" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C962" s="0" t="s">
+      <c r="G962" s="0" t="s">
         <v>4727</v>
       </c>
-      <c r="D962" s="0" t="s">
-        <v>3920</v>
-      </c>
-      <c r="I962" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="K962" s="0" t="n">
-        <v>11</v>
+      <c r="H962" s="0" t="s">
+        <v>4727</v>
       </c>
       <c r="L962" s="0" t="s">
         <v>0</v>
@@ -40182,107 +40167,113 @@
       <c r="M962" s="0" t="s">
         <v>4728</v>
       </c>
-      <c r="N962" s="0" t="s">
-        <v>4729</v>
-      </c>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A963" s="0" t="s">
+        <v>4729</v>
+      </c>
+      <c r="B963" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C963" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D963" s="0" t="s">
         <v>4730</v>
       </c>
-      <c r="E963" s="0" t="s">
+      <c r="I963" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="L963" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M963" s="0" t="s">
         <v>4731</v>
       </c>
-      <c r="G963" s="0" t="s">
+      <c r="N963" s="0" t="s">
         <v>4732</v>
-      </c>
-      <c r="H963" s="0" t="s">
-        <v>4732</v>
-      </c>
-      <c r="L963" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M963" s="0" t="s">
-        <v>4733</v>
       </c>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A964" s="0" t="s">
+        <v>4733</v>
+      </c>
+      <c r="C964" s="0" t="s">
         <v>4734</v>
-      </c>
-      <c r="B964" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C964" s="0" t="s">
-        <v>59</v>
       </c>
       <c r="D964" s="0" t="s">
         <v>4735</v>
       </c>
-      <c r="I964" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="L964" s="0" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="M964" s="0" t="s">
         <v>4736</v>
       </c>
-      <c r="N964" s="0" t="s">
-        <v>4737</v>
-      </c>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A965" s="0" t="s">
+        <v>4737</v>
+      </c>
+      <c r="D965" s="0" t="s">
         <v>4738</v>
       </c>
-      <c r="C965" s="0" t="s">
+      <c r="L965" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M965" s="0" t="s">
         <v>4739</v>
-      </c>
-      <c r="D965" s="0" t="s">
-        <v>4740</v>
-      </c>
-      <c r="L965" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M965" s="0" t="s">
-        <v>4741</v>
       </c>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A966" s="0" t="s">
+        <v>4740</v>
+      </c>
+      <c r="B966" s="0" t="s">
+        <v>596</v>
+      </c>
+      <c r="C966" s="0" t="s">
+        <v>3572</v>
+      </c>
+      <c r="D966" s="0" t="s">
+        <v>4741</v>
+      </c>
+      <c r="F966" s="0" t="s">
         <v>4742</v>
       </c>
-      <c r="D966" s="0" t="s">
+      <c r="L966" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M966" s="0" t="s">
         <v>4743</v>
-      </c>
-      <c r="L966" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M966" s="0" t="s">
-        <v>4744</v>
       </c>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A967" s="0" t="s">
+        <v>4744</v>
+      </c>
+      <c r="B967" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C967" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D967" s="0" t="s">
         <v>4745</v>
       </c>
-      <c r="B967" s="0" t="s">
-        <v>596</v>
-      </c>
-      <c r="C967" s="0" t="s">
-        <v>3572</v>
-      </c>
-      <c r="D967" s="0" t="s">
+      <c r="I967" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="L967" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="M967" s="9" t="s">
         <v>4746</v>
       </c>
-      <c r="F967" s="0" t="s">
+      <c r="N967" s="0" t="s">
         <v>4747</v>
       </c>
-      <c r="L967" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M967" s="0" t="s">
+      <c r="O967" s="0" t="s">
         <v>4748</v>
       </c>
     </row>
@@ -40294,54 +40285,48 @@
         <v>58</v>
       </c>
       <c r="C968" s="0" t="s">
-        <v>149</v>
+        <v>4750</v>
       </c>
       <c r="D968" s="0" t="s">
-        <v>4750</v>
+        <v>4751</v>
       </c>
       <c r="I968" s="0" t="s">
-        <v>151</v>
+        <v>76</v>
+      </c>
+      <c r="K968" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="L968" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="M968" s="9" t="s">
-        <v>4751</v>
-      </c>
-      <c r="N968" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M968" s="0" t="s">
         <v>4752</v>
       </c>
-      <c r="O968" s="0" t="s">
+    </row>
+    <row r="969" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A969" s="0" t="s">
         <v>4753</v>
       </c>
-    </row>
-    <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A969" s="0" t="s">
+      <c r="B969" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D969" s="0" t="s">
         <v>4754</v>
       </c>
-      <c r="B969" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C969" s="0" t="s">
+      <c r="L969" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="M969" s="9" t="s">
         <v>4755</v>
       </c>
-      <c r="D969" s="0" t="s">
+      <c r="N969" s="12" t="s">
         <v>4756</v>
       </c>
-      <c r="I969" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="K969" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="L969" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M969" s="0" t="s">
+      <c r="O969" s="0" t="s">
         <v>4757</v>
       </c>
     </row>
-    <row r="970" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A970" s="0" t="s">
         <v>4758</v>
       </c>
@@ -40351,13 +40336,19 @@
       <c r="D970" s="0" t="s">
         <v>4759</v>
       </c>
+      <c r="F970" s="0" t="s">
+        <v>2797</v>
+      </c>
+      <c r="I970" s="0" t="s">
+        <v>652</v>
+      </c>
       <c r="L970" s="0" t="s">
-        <v>511</v>
+        <v>40</v>
       </c>
       <c r="M970" s="9" t="s">
         <v>4760</v>
       </c>
-      <c r="N970" s="12" t="s">
+      <c r="N970" s="0" t="s">
         <v>4761</v>
       </c>
       <c r="O970" s="0" t="s">
@@ -40369,53 +40360,47 @@
         <v>4763</v>
       </c>
       <c r="B971" s="0" t="s">
-        <v>23</v>
+        <v>58</v>
+      </c>
+      <c r="C971" s="0" t="s">
+        <v>4764</v>
       </c>
       <c r="D971" s="0" t="s">
-        <v>4764</v>
-      </c>
-      <c r="F971" s="0" t="s">
-        <v>2797</v>
+        <v>4765</v>
       </c>
       <c r="I971" s="0" t="s">
-        <v>652</v>
+        <v>76</v>
+      </c>
+      <c r="K971" s="0" t="n">
+        <v>15</v>
       </c>
       <c r="L971" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="M971" s="9" t="s">
-        <v>4765</v>
-      </c>
-      <c r="N971" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M971" s="0" t="s">
         <v>4766</v>
-      </c>
-      <c r="O971" s="0" t="s">
-        <v>4767</v>
       </c>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A972" s="0" t="s">
+        <v>4767</v>
+      </c>
+      <c r="B972" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D972" s="0" t="s">
         <v>4768</v>
       </c>
-      <c r="B972" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C972" s="0" t="s">
+      <c r="E972" s="0" t="s">
         <v>4769</v>
       </c>
-      <c r="D972" s="0" t="s">
+      <c r="L972" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="M972" s="0" t="s">
         <v>4770</v>
       </c>
-      <c r="I972" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="K972" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="L972" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M972" s="0" t="s">
+      <c r="O972" s="0" t="s">
         <v>4771</v>
       </c>
     </row>
@@ -40429,78 +40414,78 @@
       <c r="D973" s="0" t="s">
         <v>4773</v>
       </c>
-      <c r="E973" s="0" t="s">
+      <c r="F973" s="0" t="s">
+        <v>4773</v>
+      </c>
+      <c r="I973" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="K973" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L973" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="M973" s="0" t="s">
+        <v>4773</v>
+      </c>
+      <c r="O973" s="0" t="s">
         <v>4774</v>
-      </c>
-      <c r="L973" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="M973" s="0" t="s">
-        <v>4775</v>
-      </c>
-      <c r="O973" s="0" t="s">
-        <v>4776</v>
       </c>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A974" s="0" t="s">
+        <v>4775</v>
+      </c>
+      <c r="B974" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C974" s="3"/>
+      <c r="D974" s="3" t="s">
+        <v>4776</v>
+      </c>
+      <c r="E974" s="3" t="s">
         <v>4777</v>
       </c>
-      <c r="B974" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D974" s="0" t="s">
+      <c r="F974" s="3"/>
+      <c r="G974" s="3"/>
+      <c r="H974" s="3"/>
+      <c r="I974" s="3"/>
+      <c r="J974" s="3"/>
+      <c r="K974" s="3"/>
+      <c r="L974" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M974" s="4" t="s">
         <v>4778</v>
       </c>
-      <c r="F974" s="0" t="s">
-        <v>4778</v>
-      </c>
-      <c r="I974" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="K974" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L974" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="M974" s="0" t="s">
-        <v>4778</v>
-      </c>
-      <c r="O974" s="0" t="s">
+      <c r="N974" s="3" t="s">
         <v>4779</v>
+      </c>
+      <c r="O974" s="3" t="s">
+        <v>4780</v>
       </c>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A975" s="0" t="s">
-        <v>4780</v>
-      </c>
-      <c r="B975" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C975" s="3"/>
-      <c r="D975" s="3" t="s">
         <v>4781</v>
       </c>
-      <c r="E975" s="3" t="s">
+      <c r="B975" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E975" s="0" t="s">
         <v>4782</v>
       </c>
-      <c r="F975" s="3"/>
-      <c r="G975" s="3"/>
-      <c r="H975" s="3"/>
-      <c r="I975" s="3"/>
-      <c r="J975" s="3"/>
-      <c r="K975" s="3"/>
-      <c r="L975" s="3" t="s">
+      <c r="L975" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="M975" s="4" t="s">
+      <c r="M975" s="9" t="s">
         <v>4783</v>
       </c>
-      <c r="N975" s="3" t="s">
+      <c r="N975" s="0" t="s">
         <v>4784</v>
       </c>
-      <c r="O975" s="3" t="s">
+      <c r="O975" s="0" t="s">
         <v>4785</v>
       </c>
     </row>
@@ -40511,148 +40496,151 @@
       <c r="B976" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E976" s="0" t="s">
+      <c r="D976" s="0" t="s">
         <v>4787</v>
       </c>
+      <c r="I976" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="K976" s="0" t="n">
+        <v>12</v>
+      </c>
       <c r="L976" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="M976" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="M976" s="0" t="s">
         <v>4788</v>
       </c>
-      <c r="N976" s="0" t="s">
+      <c r="O976" s="0" t="s">
         <v>4789</v>
-      </c>
-      <c r="O976" s="0" t="s">
-        <v>4790</v>
       </c>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A977" s="0" t="s">
+        <v>4790</v>
+      </c>
+      <c r="D977" s="0" t="s">
         <v>4791</v>
       </c>
-      <c r="B977" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D977" s="0" t="s">
+      <c r="L977" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M977" s="0" t="s">
         <v>4792</v>
-      </c>
-      <c r="I977" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="K977" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="L977" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="M977" s="0" t="s">
-        <v>4793</v>
-      </c>
-      <c r="O977" s="0" t="s">
-        <v>4794</v>
       </c>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A978" s="0" t="s">
+        <v>4793</v>
+      </c>
+      <c r="C978" s="0" t="s">
+        <v>4794</v>
+      </c>
+      <c r="D978" s="0" t="s">
         <v>4795</v>
       </c>
-      <c r="D978" s="0" t="s">
+      <c r="L978" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M978" s="0" t="s">
         <v>4796</v>
       </c>
-      <c r="L978" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M978" s="0" t="s">
+    </row>
+    <row r="979" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A979" s="0" t="s">
         <v>4797</v>
       </c>
-    </row>
-    <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A979" s="0" t="s">
+      <c r="B979" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D979" s="0" t="s">
         <v>4798</v>
       </c>
-      <c r="C979" s="0" t="s">
+      <c r="E979" s="0" t="s">
         <v>4799</v>
       </c>
-      <c r="D979" s="0" t="s">
+      <c r="L979" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="M979" s="21" t="s">
         <v>4800</v>
       </c>
-      <c r="L979" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M979" s="0" t="s">
+      <c r="N979" s="5" t="s">
         <v>4801</v>
       </c>
-    </row>
-    <row r="980" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O979" s="5" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A980" s="0" t="s">
-        <v>4802</v>
+        <v>4803</v>
       </c>
       <c r="B980" s="0" t="s">
         <v>23</v>
       </c>
       <c r="D980" s="0" t="s">
-        <v>4803</v>
+        <v>4804</v>
       </c>
       <c r="E980" s="0" t="s">
-        <v>4804</v>
+        <v>4805</v>
+      </c>
+      <c r="F980" s="0" t="s">
+        <v>4806</v>
+      </c>
+      <c r="G980" s="0" t="s">
+        <v>4807</v>
+      </c>
+      <c r="I980" s="0" t="s">
+        <v>145</v>
       </c>
       <c r="L980" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="M980" s="21" t="s">
-        <v>4805</v>
-      </c>
-      <c r="N980" s="5" t="s">
-        <v>4806</v>
-      </c>
-      <c r="O980" s="5" t="s">
-        <v>4807</v>
+      <c r="M980" s="9" t="s">
+        <v>4808</v>
+      </c>
+      <c r="N980" s="0" t="s">
+        <v>4809</v>
+      </c>
+      <c r="O980" s="0" t="s">
+        <v>4810</v>
       </c>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A981" s="0" t="s">
-        <v>4808</v>
+        <v>4811</v>
       </c>
       <c r="B981" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="C981" s="0" t="s">
+        <v>4812</v>
+      </c>
       <c r="D981" s="0" t="s">
-        <v>4809</v>
-      </c>
-      <c r="E981" s="0" t="s">
-        <v>4810</v>
-      </c>
-      <c r="F981" s="0" t="s">
-        <v>4811</v>
-      </c>
-      <c r="G981" s="0" t="s">
-        <v>4812</v>
+        <v>4813</v>
       </c>
       <c r="I981" s="0" t="s">
-        <v>145</v>
+        <v>226</v>
+      </c>
+      <c r="K981" s="0" t="n">
+        <v>37</v>
       </c>
       <c r="L981" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="M981" s="9" t="s">
-        <v>4813</v>
+        <v>52</v>
+      </c>
+      <c r="M981" s="0" t="s">
+        <v>4814</v>
       </c>
       <c r="N981" s="0" t="s">
-        <v>4814</v>
+        <v>4815</v>
       </c>
       <c r="O981" s="0" t="s">
-        <v>4815</v>
+        <v>4816</v>
       </c>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A982" s="0" t="s">
-        <v>4816</v>
-      </c>
-      <c r="B982" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C982" s="0" t="s">
         <v>4817</v>
       </c>
       <c r="D982" s="0" t="s">
@@ -40662,10 +40650,10 @@
         <v>226</v>
       </c>
       <c r="K982" s="0" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L982" s="0" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="M982" s="0" t="s">
         <v>4819</v>
@@ -40673,30 +40661,33 @@
       <c r="N982" s="0" t="s">
         <v>4820</v>
       </c>
-      <c r="O982" s="0" t="s">
-        <v>4821</v>
-      </c>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A983" s="0" t="s">
+        <v>4821</v>
+      </c>
+      <c r="B983" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D983" s="0" t="s">
         <v>4822</v>
       </c>
-      <c r="D983" s="0" t="s">
+      <c r="E983" s="0" t="s">
         <v>4823</v>
       </c>
       <c r="I983" s="0" t="s">
         <v>226</v>
       </c>
       <c r="K983" s="0" t="n">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="L983" s="0" t="s">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="M983" s="0" t="s">
         <v>4824</v>
       </c>
-      <c r="N983" s="0" t="s">
+      <c r="O983" s="0" t="s">
         <v>4825</v>
       </c>
     </row>
@@ -40707,559 +40698,550 @@
       <c r="B984" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="C984" s="0" t="s">
+        <v>4827</v>
+      </c>
       <c r="D984" s="0" t="s">
-        <v>4827</v>
-      </c>
-      <c r="E984" s="0" t="s">
         <v>4828</v>
       </c>
-      <c r="I984" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="K984" s="0" t="n">
-        <v>61</v>
+      <c r="F984" s="0" t="s">
+        <v>4829</v>
       </c>
       <c r="L984" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="M984" s="0" t="s">
-        <v>4829</v>
+        <v>40</v>
+      </c>
+      <c r="M984" s="9" t="s">
+        <v>4830</v>
+      </c>
+      <c r="N984" s="11" t="s">
+        <v>4831</v>
       </c>
       <c r="O984" s="0" t="s">
-        <v>4830</v>
+        <v>4832</v>
       </c>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A985" s="0" t="s">
-        <v>4831</v>
+        <v>4833</v>
       </c>
       <c r="B985" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C985" s="0" t="s">
-        <v>4832</v>
-      </c>
       <c r="D985" s="0" t="s">
-        <v>4833</v>
+        <v>4834</v>
       </c>
       <c r="F985" s="0" t="s">
-        <v>4834</v>
+        <v>4835</v>
       </c>
       <c r="L985" s="0" t="s">
         <v>40</v>
       </c>
       <c r="M985" s="9" t="s">
-        <v>4835</v>
-      </c>
-      <c r="N985" s="11" t="s">
         <v>4836</v>
       </c>
+      <c r="N985" s="0" t="s">
+        <v>4837</v>
+      </c>
       <c r="O985" s="0" t="s">
-        <v>4837</v>
+        <v>4838</v>
       </c>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A986" s="0" t="s">
-        <v>4838</v>
+        <v>4839</v>
       </c>
       <c r="B986" s="0" t="s">
         <v>23</v>
       </c>
       <c r="D986" s="0" t="s">
-        <v>4839</v>
+        <v>4840</v>
+      </c>
+      <c r="E986" s="0" t="s">
+        <v>4841</v>
       </c>
       <c r="F986" s="0" t="s">
-        <v>4840</v>
+        <v>4842</v>
+      </c>
+      <c r="I986" s="0" t="s">
+        <v>226</v>
       </c>
       <c r="L986" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="M986" s="9" t="s">
-        <v>4841</v>
-      </c>
-      <c r="N986" s="0" t="s">
-        <v>4842</v>
+        <v>735</v>
+      </c>
+      <c r="M986" s="0" t="s">
+        <v>4843</v>
       </c>
       <c r="O986" s="0" t="s">
-        <v>4843</v>
+        <v>4844</v>
       </c>
     </row>
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A987" s="0" t="s">
-        <v>4844</v>
+        <v>4845</v>
       </c>
       <c r="B987" s="0" t="s">
         <v>23</v>
       </c>
       <c r="D987" s="0" t="s">
-        <v>4845</v>
-      </c>
-      <c r="E987" s="0" t="s">
         <v>4846</v>
       </c>
-      <c r="F987" s="0" t="s">
+      <c r="I987" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="L987" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="M987" s="0" t="s">
         <v>4847</v>
       </c>
-      <c r="I987" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="L987" s="0" t="s">
-        <v>735</v>
-      </c>
-      <c r="M987" s="0" t="s">
+      <c r="O987" s="0" t="s">
         <v>4848</v>
-      </c>
-      <c r="O987" s="0" t="s">
-        <v>4849</v>
       </c>
     </row>
     <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A988" s="0" t="s">
+        <v>4849</v>
+      </c>
+      <c r="B988" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D988" s="0" t="s">
         <v>4850</v>
       </c>
-      <c r="B988" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D988" s="0" t="s">
+      <c r="I988" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="K988" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L988" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="M988" s="0" t="s">
         <v>4851</v>
       </c>
-      <c r="I988" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="L988" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="M988" s="0" t="s">
+      <c r="O988" s="0" t="s">
         <v>4852</v>
-      </c>
-      <c r="O988" s="0" t="s">
-        <v>4853</v>
       </c>
     </row>
     <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A989" s="0" t="s">
+        <v>4853</v>
+      </c>
+      <c r="D989" s="0" t="s">
         <v>4854</v>
-      </c>
-      <c r="B989" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D989" s="0" t="s">
-        <v>4855</v>
       </c>
       <c r="I989" s="0" t="s">
         <v>76</v>
       </c>
       <c r="K989" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L989" s="0" t="s">
-        <v>254</v>
+        <v>0</v>
       </c>
       <c r="M989" s="0" t="s">
+        <v>4855</v>
+      </c>
+      <c r="N989" s="0" t="s">
         <v>4856</v>
-      </c>
-      <c r="O989" s="0" t="s">
-        <v>4857</v>
       </c>
     </row>
     <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A990" s="0" t="s">
+        <v>4857</v>
+      </c>
+      <c r="D990" s="0" t="s">
         <v>4858</v>
-      </c>
-      <c r="D990" s="0" t="s">
-        <v>4859</v>
       </c>
       <c r="I990" s="0" t="s">
         <v>76</v>
       </c>
       <c r="K990" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L990" s="0" t="s">
         <v>0</v>
       </c>
       <c r="M990" s="0" t="s">
+        <v>4859</v>
+      </c>
+      <c r="N990" s="0" t="s">
         <v>4860</v>
-      </c>
-      <c r="N990" s="0" t="s">
-        <v>4861</v>
       </c>
     </row>
     <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A991" s="0" t="s">
+        <v>4861</v>
+      </c>
+      <c r="B991" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D991" s="0" t="s">
         <v>4862</v>
       </c>
-      <c r="D991" s="0" t="s">
+      <c r="E991" s="0" t="s">
         <v>4863</v>
       </c>
-      <c r="I991" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="K991" s="0" t="n">
-        <v>5</v>
+      <c r="F991" s="0" t="s">
+        <v>4864</v>
       </c>
       <c r="L991" s="0" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="M991" s="0" t="s">
-        <v>4864</v>
-      </c>
-      <c r="N991" s="0" t="s">
         <v>4865</v>
+      </c>
+      <c r="O991" s="0" t="s">
+        <v>4866</v>
       </c>
     </row>
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A992" s="0" t="s">
-        <v>4866</v>
-      </c>
-      <c r="B992" s="0" t="s">
-        <v>23</v>
+        <v>4867</v>
       </c>
       <c r="D992" s="0" t="s">
-        <v>4867</v>
-      </c>
-      <c r="E992" s="0" t="s">
         <v>4868</v>
       </c>
-      <c r="F992" s="0" t="s">
+      <c r="L992" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M992" s="0" t="s">
         <v>4869</v>
-      </c>
-      <c r="L992" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="M992" s="0" t="s">
-        <v>4870</v>
-      </c>
-      <c r="O992" s="0" t="s">
-        <v>4871</v>
       </c>
     </row>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A993" s="0" t="s">
+        <v>4870</v>
+      </c>
+      <c r="D993" s="0" t="s">
+        <v>4871</v>
+      </c>
+      <c r="L993" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M993" s="0" t="s">
         <v>4872</v>
-      </c>
-      <c r="D993" s="0" t="s">
-        <v>4873</v>
-      </c>
-      <c r="L993" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M993" s="0" t="s">
-        <v>4874</v>
       </c>
     </row>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A994" s="0" t="s">
+        <v>4873</v>
+      </c>
+      <c r="C994" s="0" t="s">
+        <v>4874</v>
+      </c>
+      <c r="D994" s="0" t="s">
         <v>4875</v>
       </c>
-      <c r="D994" s="0" t="s">
+      <c r="L994" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M994" s="0" t="s">
         <v>4876</v>
-      </c>
-      <c r="L994" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M994" s="0" t="s">
-        <v>4877</v>
       </c>
     </row>
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A995" s="0" t="s">
+        <v>4877</v>
+      </c>
+      <c r="B995" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C995" s="0" t="s">
         <v>4878</v>
       </c>
-      <c r="C995" s="0" t="s">
+      <c r="D995" s="0" t="s">
+        <v>4875</v>
+      </c>
+      <c r="I995" s="0" t="s">
+        <v>3567</v>
+      </c>
+      <c r="K995" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L995" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M995" s="0" t="s">
         <v>4879</v>
-      </c>
-      <c r="D995" s="0" t="s">
-        <v>4880</v>
-      </c>
-      <c r="L995" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M995" s="0" t="s">
-        <v>4881</v>
       </c>
     </row>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A996" s="0" t="s">
+        <v>4880</v>
+      </c>
+      <c r="C996" s="0" t="s">
+        <v>4881</v>
+      </c>
+      <c r="D996" s="0" t="s">
         <v>4882</v>
       </c>
-      <c r="B996" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C996" s="0" t="s">
+      <c r="L996" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M996" s="0" t="s">
         <v>4883</v>
-      </c>
-      <c r="D996" s="0" t="s">
-        <v>4880</v>
-      </c>
-      <c r="I996" s="0" t="s">
-        <v>3567</v>
-      </c>
-      <c r="K996" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L996" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M996" s="0" t="s">
-        <v>4884</v>
       </c>
     </row>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A997" s="0" t="s">
+        <v>4884</v>
+      </c>
+      <c r="B997" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C997" s="0" t="s">
         <v>4885</v>
       </c>
-      <c r="C997" s="0" t="s">
+      <c r="D997" s="0" t="s">
+        <v>4882</v>
+      </c>
+      <c r="I997" s="0" t="s">
+        <v>3567</v>
+      </c>
+      <c r="K997" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L997" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M997" s="0" t="s">
         <v>4886</v>
-      </c>
-      <c r="D997" s="0" t="s">
-        <v>4887</v>
-      </c>
-      <c r="L997" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M997" s="0" t="s">
-        <v>4888</v>
       </c>
     </row>
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A998" s="0" t="s">
+        <v>4887</v>
+      </c>
+      <c r="C998" s="0" t="s">
+        <v>4888</v>
+      </c>
+      <c r="D998" s="0" t="s">
         <v>4889</v>
       </c>
-      <c r="B998" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C998" s="0" t="s">
+      <c r="L998" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M998" s="0" t="s">
         <v>4890</v>
-      </c>
-      <c r="D998" s="0" t="s">
-        <v>4887</v>
-      </c>
-      <c r="I998" s="0" t="s">
-        <v>3567</v>
-      </c>
-      <c r="K998" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L998" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M998" s="0" t="s">
-        <v>4891</v>
       </c>
     </row>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A999" s="0" t="s">
+        <v>4891</v>
+      </c>
+      <c r="B999" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C999" s="0" t="s">
         <v>4892</v>
       </c>
-      <c r="C999" s="0" t="s">
+      <c r="D999" s="0" t="s">
+        <v>4889</v>
+      </c>
+      <c r="I999" s="0" t="s">
+        <v>3567</v>
+      </c>
+      <c r="K999" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L999" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M999" s="0" t="s">
         <v>4893</v>
-      </c>
-      <c r="D999" s="0" t="s">
-        <v>4894</v>
-      </c>
-      <c r="L999" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M999" s="0" t="s">
-        <v>4895</v>
       </c>
     </row>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1000" s="0" t="s">
+        <v>4894</v>
+      </c>
+      <c r="C1000" s="0" t="s">
+        <v>4895</v>
+      </c>
+      <c r="D1000" s="0" t="s">
         <v>4896</v>
       </c>
-      <c r="B1000" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1000" s="0" t="s">
+      <c r="L1000" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1000" s="0" t="s">
         <v>4897</v>
-      </c>
-      <c r="D1000" s="0" t="s">
-        <v>4894</v>
-      </c>
-      <c r="I1000" s="0" t="s">
-        <v>3567</v>
-      </c>
-      <c r="K1000" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L1000" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1000" s="0" t="s">
-        <v>4898</v>
       </c>
     </row>
     <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1001" s="0" t="s">
+        <v>4898</v>
+      </c>
+      <c r="B1001" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1001" s="0" t="s">
         <v>4899</v>
       </c>
-      <c r="C1001" s="0" t="s">
+      <c r="D1001" s="0" t="s">
+        <v>4896</v>
+      </c>
+      <c r="I1001" s="0" t="s">
+        <v>3567</v>
+      </c>
+      <c r="K1001" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L1001" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1001" s="0" t="s">
         <v>4900</v>
-      </c>
-      <c r="D1001" s="0" t="s">
-        <v>4901</v>
-      </c>
-      <c r="L1001" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1001" s="0" t="s">
-        <v>4902</v>
       </c>
     </row>
     <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1002" s="0" t="s">
+        <v>4901</v>
+      </c>
+      <c r="C1002" s="0" t="s">
+        <v>4902</v>
+      </c>
+      <c r="D1002" s="0" t="s">
         <v>4903</v>
       </c>
-      <c r="B1002" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1002" s="0" t="s">
+      <c r="L1002" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1002" s="0" t="s">
         <v>4904</v>
-      </c>
-      <c r="D1002" s="0" t="s">
-        <v>4901</v>
-      </c>
-      <c r="I1002" s="0" t="s">
-        <v>3567</v>
-      </c>
-      <c r="K1002" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="L1002" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1002" s="0" t="s">
-        <v>4905</v>
       </c>
     </row>
     <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1003" s="0" t="s">
+        <v>4905</v>
+      </c>
+      <c r="B1003" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1003" s="0" t="s">
         <v>4906</v>
       </c>
-      <c r="C1003" s="0" t="s">
+      <c r="D1003" s="0" t="s">
+        <v>4903</v>
+      </c>
+      <c r="I1003" s="0" t="s">
+        <v>3567</v>
+      </c>
+      <c r="K1003" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L1003" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1003" s="0" t="s">
         <v>4907</v>
-      </c>
-      <c r="D1003" s="0" t="s">
-        <v>4908</v>
-      </c>
-      <c r="L1003" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1003" s="0" t="s">
-        <v>4909</v>
       </c>
     </row>
     <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1004" s="0" t="s">
+        <v>4908</v>
+      </c>
+      <c r="C1004" s="0" t="s">
+        <v>4909</v>
+      </c>
+      <c r="D1004" s="0" t="s">
         <v>4910</v>
       </c>
-      <c r="B1004" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1004" s="0" t="s">
+      <c r="L1004" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1004" s="0" t="s">
         <v>4911</v>
-      </c>
-      <c r="D1004" s="0" t="s">
-        <v>4908</v>
-      </c>
-      <c r="I1004" s="0" t="s">
-        <v>3567</v>
-      </c>
-      <c r="K1004" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L1004" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1004" s="0" t="s">
-        <v>4912</v>
       </c>
     </row>
     <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1005" s="0" t="s">
+        <v>4912</v>
+      </c>
+      <c r="B1005" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1005" s="0" t="s">
         <v>4913</v>
       </c>
-      <c r="C1005" s="0" t="s">
+      <c r="D1005" s="0" t="s">
+        <v>4910</v>
+      </c>
+      <c r="I1005" s="0" t="s">
+        <v>3567</v>
+      </c>
+      <c r="K1005" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L1005" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1005" s="0" t="s">
         <v>4914</v>
-      </c>
-      <c r="D1005" s="0" t="s">
-        <v>4915</v>
-      </c>
-      <c r="L1005" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1005" s="0" t="s">
-        <v>4916</v>
       </c>
     </row>
     <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1006" s="0" t="s">
+        <v>4915</v>
+      </c>
+      <c r="C1006" s="0" t="s">
+        <v>4916</v>
+      </c>
+      <c r="D1006" s="0" t="s">
         <v>4917</v>
       </c>
-      <c r="B1006" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1006" s="0" t="s">
+      <c r="L1006" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1006" s="0" t="s">
         <v>4918</v>
-      </c>
-      <c r="D1006" s="0" t="s">
-        <v>4915</v>
-      </c>
-      <c r="I1006" s="0" t="s">
-        <v>3567</v>
-      </c>
-      <c r="K1006" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L1006" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1006" s="0" t="s">
-        <v>4919</v>
       </c>
     </row>
     <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1007" s="0" t="s">
+        <v>4919</v>
+      </c>
+      <c r="B1007" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1007" s="0" t="s">
         <v>4920</v>
       </c>
-      <c r="C1007" s="0" t="s">
+      <c r="D1007" s="0" t="s">
+        <v>4917</v>
+      </c>
+      <c r="I1007" s="0" t="s">
+        <v>3567</v>
+      </c>
+      <c r="K1007" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L1007" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1007" s="0" t="s">
         <v>4921</v>
-      </c>
-      <c r="D1007" s="0" t="s">
-        <v>4922</v>
-      </c>
-      <c r="L1007" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1007" s="0" t="s">
-        <v>4923</v>
       </c>
     </row>
     <row r="1008" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1008" s="0" t="s">
+        <v>4922</v>
+      </c>
+      <c r="D1008" s="0" t="s">
+        <v>4923</v>
+      </c>
+      <c r="L1008" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1008" s="0" t="s">
         <v>4924</v>
       </c>
-      <c r="B1008" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1008" s="0" t="s">
+      <c r="N1008" s="0" t="s">
         <v>4925</v>
       </c>
-      <c r="D1008" s="0" t="s">
-        <v>4922</v>
-      </c>
-      <c r="I1008" s="0" t="s">
-        <v>3567</v>
-      </c>
-      <c r="K1008" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="L1008" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1008" s="0" t="s">
+      <c r="O1008" s="0" t="s">
         <v>4926</v>
       </c>
     </row>
@@ -41267,617 +41249,623 @@
       <c r="A1009" s="0" t="s">
         <v>4927</v>
       </c>
+      <c r="B1009" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1009" s="0" t="s">
+        <v>4928</v>
+      </c>
       <c r="D1009" s="0" t="s">
-        <v>4928</v>
+        <v>4929</v>
+      </c>
+      <c r="I1009" s="0" t="s">
+        <v>2002</v>
+      </c>
+      <c r="K1009" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="L1009" s="0" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="M1009" s="0" t="s">
-        <v>4929</v>
-      </c>
-      <c r="N1009" s="0" t="s">
         <v>4930</v>
-      </c>
-      <c r="O1009" s="0" t="s">
-        <v>4931</v>
       </c>
     </row>
     <row r="1010" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1010" s="0" t="s">
-        <v>4932</v>
+        <v>4931</v>
       </c>
       <c r="B1010" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1010" s="0" t="s">
+        <v>4932</v>
+      </c>
+      <c r="D1010" s="0" t="s">
         <v>4933</v>
-      </c>
-      <c r="D1010" s="0" t="s">
-        <v>4934</v>
       </c>
       <c r="I1010" s="0" t="s">
         <v>2002</v>
       </c>
       <c r="K1010" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L1010" s="0" t="s">
         <v>0</v>
       </c>
       <c r="M1010" s="0" t="s">
-        <v>4935</v>
+        <v>4934</v>
       </c>
     </row>
     <row r="1011" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1011" s="0" t="s">
-        <v>4936</v>
+        <v>4935</v>
       </c>
       <c r="B1011" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1011" s="0" t="s">
+        <v>4936</v>
+      </c>
+      <c r="D1011" s="0" t="s">
         <v>4937</v>
-      </c>
-      <c r="D1011" s="0" t="s">
-        <v>4938</v>
       </c>
       <c r="I1011" s="0" t="s">
         <v>2002</v>
       </c>
       <c r="K1011" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L1011" s="0" t="s">
         <v>0</v>
       </c>
       <c r="M1011" s="0" t="s">
-        <v>4939</v>
+        <v>4938</v>
       </c>
     </row>
     <row r="1012" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1012" s="0" t="s">
-        <v>4940</v>
+        <v>4939</v>
       </c>
       <c r="B1012" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1012" s="0" t="s">
+        <v>4940</v>
+      </c>
+      <c r="D1012" s="0" t="s">
         <v>4941</v>
       </c>
-      <c r="D1012" s="0" t="s">
+      <c r="I1012" s="6" t="s">
+        <v>2002</v>
+      </c>
+      <c r="K1012" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L1012" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1012" s="0" t="s">
         <v>4942</v>
-      </c>
-      <c r="I1012" s="0" t="s">
-        <v>2002</v>
-      </c>
-      <c r="K1012" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L1012" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1012" s="0" t="s">
-        <v>4943</v>
       </c>
     </row>
     <row r="1013" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1013" s="0" t="s">
-        <v>4944</v>
+        <v>4943</v>
       </c>
       <c r="B1013" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1013" s="0" t="s">
+        <v>4944</v>
+      </c>
+      <c r="D1013" s="0" t="s">
         <v>4945</v>
       </c>
-      <c r="D1013" s="0" t="s">
+      <c r="I1013" s="0" t="s">
+        <v>2002</v>
+      </c>
+      <c r="K1013" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L1013" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1013" s="0" t="s">
         <v>4946</v>
-      </c>
-      <c r="I1013" s="6" t="s">
-        <v>2002</v>
-      </c>
-      <c r="K1013" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="L1013" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1013" s="0" t="s">
-        <v>4947</v>
       </c>
     </row>
     <row r="1014" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1014" s="0" t="s">
-        <v>4948</v>
+        <v>4947</v>
       </c>
       <c r="B1014" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1014" s="0" t="s">
+        <v>4948</v>
+      </c>
+      <c r="D1014" s="0" t="s">
         <v>4949</v>
       </c>
-      <c r="D1014" s="0" t="s">
+      <c r="I1014" s="6" t="s">
+        <v>2002</v>
+      </c>
+      <c r="K1014" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L1014" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1014" s="0" t="s">
         <v>4950</v>
-      </c>
-      <c r="I1014" s="0" t="s">
-        <v>2002</v>
-      </c>
-      <c r="K1014" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L1014" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1014" s="0" t="s">
-        <v>4951</v>
       </c>
     </row>
     <row r="1015" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1015" s="0" t="s">
-        <v>4952</v>
+        <v>4951</v>
       </c>
       <c r="B1015" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1015" s="0" t="s">
+        <v>4952</v>
+      </c>
+      <c r="D1015" s="0" t="s">
         <v>4953</v>
       </c>
-      <c r="D1015" s="0" t="s">
+      <c r="I1015" s="0" t="s">
+        <v>2002</v>
+      </c>
+      <c r="K1015" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L1015" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1015" s="0" t="s">
         <v>4954</v>
-      </c>
-      <c r="I1015" s="6" t="s">
-        <v>2002</v>
-      </c>
-      <c r="K1015" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L1015" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1015" s="0" t="s">
-        <v>4955</v>
       </c>
     </row>
     <row r="1016" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1016" s="0" t="s">
-        <v>4956</v>
+        <v>4955</v>
       </c>
       <c r="B1016" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1016" s="0" t="s">
+        <v>4956</v>
+      </c>
+      <c r="D1016" s="0" t="s">
         <v>4957</v>
       </c>
-      <c r="D1016" s="0" t="s">
+      <c r="I1016" s="6" t="s">
+        <v>2002</v>
+      </c>
+      <c r="K1016" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L1016" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1016" s="0" t="s">
         <v>4958</v>
-      </c>
-      <c r="I1016" s="0" t="s">
-        <v>2002</v>
-      </c>
-      <c r="K1016" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="L1016" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1016" s="0" t="s">
-        <v>4959</v>
       </c>
     </row>
     <row r="1017" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1017" s="0" t="s">
-        <v>4960</v>
+        <v>4959</v>
       </c>
       <c r="B1017" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1017" s="0" t="s">
+        <v>4960</v>
+      </c>
+      <c r="D1017" s="0" t="s">
         <v>4961</v>
       </c>
-      <c r="D1017" s="0" t="s">
+      <c r="I1017" s="0" t="s">
+        <v>2002</v>
+      </c>
+      <c r="K1017" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1017" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1017" s="0" t="s">
         <v>4962</v>
-      </c>
-      <c r="I1017" s="6" t="s">
-        <v>2002</v>
-      </c>
-      <c r="K1017" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="L1017" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1017" s="0" t="s">
-        <v>4963</v>
       </c>
     </row>
     <row r="1018" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1018" s="0" t="s">
-        <v>4964</v>
+        <v>4963</v>
       </c>
       <c r="B1018" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1018" s="0" t="s">
+        <v>4964</v>
+      </c>
+      <c r="D1018" s="0" t="s">
         <v>4965</v>
       </c>
-      <c r="D1018" s="0" t="s">
+      <c r="I1018" s="6" t="s">
+        <v>2002</v>
+      </c>
+      <c r="K1018" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1018" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1018" s="0" t="s">
         <v>4966</v>
-      </c>
-      <c r="I1018" s="0" t="s">
-        <v>2002</v>
-      </c>
-      <c r="K1018" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="L1018" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1018" s="0" t="s">
-        <v>4967</v>
       </c>
     </row>
     <row r="1019" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1019" s="0" t="s">
-        <v>4968</v>
+        <v>4967</v>
       </c>
       <c r="B1019" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1019" s="0" t="s">
+        <v>4968</v>
+      </c>
+      <c r="D1019" s="0" t="s">
         <v>4969</v>
-      </c>
-      <c r="D1019" s="0" t="s">
-        <v>4970</v>
       </c>
       <c r="I1019" s="6" t="s">
         <v>2002</v>
       </c>
       <c r="K1019" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1019" s="0" t="s">
         <v>0</v>
       </c>
       <c r="M1019" s="0" t="s">
-        <v>4971</v>
+        <v>4970</v>
       </c>
     </row>
     <row r="1020" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1020" s="0" t="s">
-        <v>4972</v>
+        <v>4971</v>
       </c>
       <c r="B1020" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1020" s="0" t="s">
+        <v>4972</v>
+      </c>
+      <c r="D1020" s="0" t="s">
         <v>4973</v>
-      </c>
-      <c r="D1020" s="0" t="s">
-        <v>4974</v>
       </c>
       <c r="I1020" s="6" t="s">
         <v>2002</v>
       </c>
       <c r="K1020" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1020" s="0" t="s">
         <v>0</v>
       </c>
       <c r="M1020" s="0" t="s">
-        <v>4975</v>
+        <v>4974</v>
       </c>
     </row>
     <row r="1021" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1021" s="0" t="s">
-        <v>4976</v>
+        <v>4975</v>
       </c>
       <c r="B1021" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C1021" s="0" t="s">
+        <v>4976</v>
+      </c>
+      <c r="D1021" s="0" t="s">
         <v>4977</v>
-      </c>
-      <c r="D1021" s="0" t="s">
-        <v>4978</v>
       </c>
       <c r="I1021" s="6" t="s">
         <v>2002</v>
       </c>
       <c r="K1021" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L1021" s="0" t="s">
         <v>0</v>
       </c>
       <c r="M1021" s="0" t="s">
-        <v>4979</v>
+        <v>4978</v>
       </c>
     </row>
     <row r="1022" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1022" s="0" t="s">
+        <v>4979</v>
+      </c>
+      <c r="C1022" s="0" t="s">
         <v>4980</v>
       </c>
-      <c r="B1022" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1022" s="0" t="s">
+      <c r="D1022" s="0" t="s">
         <v>4981</v>
       </c>
-      <c r="D1022" s="0" t="s">
+      <c r="L1022" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1022" s="0" t="s">
         <v>4982</v>
-      </c>
-      <c r="I1022" s="6" t="s">
-        <v>2002</v>
-      </c>
-      <c r="K1022" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="L1022" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1022" s="0" t="s">
-        <v>4983</v>
       </c>
     </row>
     <row r="1023" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1023" s="0" t="s">
+        <v>4983</v>
+      </c>
+      <c r="C1023" s="0" t="s">
         <v>4984</v>
       </c>
-      <c r="C1023" s="0" t="s">
+      <c r="D1023" s="0" t="s">
         <v>4985</v>
       </c>
-      <c r="D1023" s="0" t="s">
+      <c r="L1023" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1023" s="0" t="s">
         <v>4986</v>
-      </c>
-      <c r="L1023" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1023" s="0" t="s">
-        <v>4987</v>
       </c>
     </row>
     <row r="1024" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1024" s="0" t="s">
+        <v>4987</v>
+      </c>
+      <c r="C1024" s="7" t="s">
         <v>4988</v>
       </c>
-      <c r="C1024" s="0" t="s">
+      <c r="D1024" s="0" t="s">
         <v>4989</v>
       </c>
-      <c r="D1024" s="0" t="s">
+      <c r="L1024" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1024" s="0" t="s">
         <v>4990</v>
-      </c>
-      <c r="L1024" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1024" s="0" t="s">
-        <v>4991</v>
       </c>
     </row>
     <row r="1025" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1025" s="0" t="s">
+        <v>4991</v>
+      </c>
+      <c r="C1025" s="7" t="s">
         <v>4992</v>
       </c>
-      <c r="C1025" s="7" t="s">
+      <c r="D1025" s="0" t="s">
         <v>4993</v>
       </c>
-      <c r="D1025" s="0" t="s">
+      <c r="L1025" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1025" s="0" t="s">
         <v>4994</v>
-      </c>
-      <c r="L1025" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1025" s="0" t="s">
-        <v>4995</v>
       </c>
     </row>
     <row r="1026" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1026" s="0" t="s">
+        <v>4995</v>
+      </c>
+      <c r="C1026" s="7" t="s">
         <v>4996</v>
       </c>
-      <c r="C1026" s="7" t="s">
+      <c r="D1026" s="0" t="s">
         <v>4997</v>
       </c>
-      <c r="D1026" s="0" t="s">
+      <c r="L1026" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1026" s="0" t="s">
         <v>4998</v>
-      </c>
-      <c r="L1026" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1026" s="0" t="s">
-        <v>4999</v>
       </c>
     </row>
     <row r="1027" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1027" s="0" t="s">
+        <v>4999</v>
+      </c>
+      <c r="C1027" s="7" t="s">
         <v>5000</v>
       </c>
-      <c r="C1027" s="7" t="s">
+      <c r="D1027" s="0" t="s">
         <v>5001</v>
       </c>
-      <c r="D1027" s="0" t="s">
+      <c r="L1027" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1027" s="0" t="s">
         <v>5002</v>
-      </c>
-      <c r="L1027" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1027" s="0" t="s">
-        <v>5003</v>
       </c>
     </row>
     <row r="1028" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1028" s="0" t="s">
+        <v>5003</v>
+      </c>
+      <c r="C1028" s="7" t="s">
         <v>5004</v>
       </c>
-      <c r="C1028" s="7" t="s">
+      <c r="D1028" s="0" t="s">
         <v>5005</v>
       </c>
-      <c r="D1028" s="0" t="s">
+      <c r="L1028" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1028" s="0" t="s">
         <v>5006</v>
-      </c>
-      <c r="L1028" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1028" s="0" t="s">
-        <v>5007</v>
       </c>
     </row>
     <row r="1029" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1029" s="0" t="s">
+        <v>5007</v>
+      </c>
+      <c r="C1029" s="7" t="s">
         <v>5008</v>
       </c>
-      <c r="C1029" s="7" t="s">
+      <c r="D1029" s="0" t="s">
         <v>5009</v>
       </c>
-      <c r="D1029" s="0" t="s">
+      <c r="L1029" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1029" s="0" t="s">
         <v>5010</v>
-      </c>
-      <c r="L1029" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1029" s="0" t="s">
-        <v>5011</v>
       </c>
     </row>
     <row r="1030" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1030" s="0" t="s">
+        <v>5011</v>
+      </c>
+      <c r="C1030" s="7" t="s">
         <v>5012</v>
       </c>
-      <c r="C1030" s="7" t="s">
+      <c r="D1030" s="0" t="s">
         <v>5013</v>
       </c>
-      <c r="D1030" s="0" t="s">
+      <c r="L1030" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1030" s="0" t="s">
         <v>5014</v>
-      </c>
-      <c r="L1030" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1030" s="0" t="s">
-        <v>5015</v>
       </c>
     </row>
     <row r="1031" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1031" s="0" t="s">
+        <v>5015</v>
+      </c>
+      <c r="C1031" s="7" t="s">
         <v>5016</v>
       </c>
-      <c r="C1031" s="7" t="s">
+      <c r="D1031" s="0" t="s">
         <v>5017</v>
       </c>
-      <c r="D1031" s="0" t="s">
+      <c r="L1031" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1031" s="0" t="s">
         <v>5018</v>
-      </c>
-      <c r="L1031" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1031" s="0" t="s">
-        <v>5019</v>
       </c>
     </row>
     <row r="1032" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1032" s="0" t="s">
+        <v>5019</v>
+      </c>
+      <c r="C1032" s="7" t="s">
         <v>5020</v>
       </c>
-      <c r="C1032" s="7" t="s">
+      <c r="D1032" s="0" t="s">
         <v>5021</v>
       </c>
-      <c r="D1032" s="0" t="s">
+      <c r="L1032" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1032" s="0" t="s">
         <v>5022</v>
-      </c>
-      <c r="L1032" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1032" s="0" t="s">
-        <v>5023</v>
       </c>
     </row>
     <row r="1033" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1033" s="0" t="s">
+        <v>5023</v>
+      </c>
+      <c r="C1033" s="7" t="s">
         <v>5024</v>
       </c>
-      <c r="C1033" s="7" t="s">
+      <c r="D1033" s="0" t="s">
         <v>5025</v>
       </c>
-      <c r="D1033" s="0" t="s">
+      <c r="L1033" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1033" s="0" t="s">
         <v>5026</v>
       </c>
-      <c r="L1033" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1033" s="0" t="s">
+    </row>
+    <row r="1034" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1034" s="0" t="s">
         <v>5027</v>
       </c>
-    </row>
-    <row r="1034" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1034" s="0" t="s">
+      <c r="B1034" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1034" s="0" t="s">
         <v>5028</v>
       </c>
-      <c r="C1034" s="7" t="s">
+      <c r="E1034" s="0" t="s">
         <v>5029</v>
       </c>
-      <c r="D1034" s="0" t="s">
+      <c r="F1034" s="0" t="s">
         <v>5030</v>
       </c>
+      <c r="I1034" s="0" t="s">
+        <v>1039</v>
+      </c>
       <c r="L1034" s="0" t="s">
-        <v>0</v>
+        <v>254</v>
       </c>
       <c r="M1034" s="0" t="s">
         <v>5031</v>
       </c>
-    </row>
-    <row r="1035" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O1034" s="0" t="s">
+        <v>5032</v>
+      </c>
+    </row>
+    <row r="1035" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1035" s="0" t="s">
-        <v>5032</v>
+        <v>4296</v>
       </c>
       <c r="B1035" s="0" t="s">
-        <v>23</v>
+        <v>596</v>
+      </c>
+      <c r="C1035" s="0" t="s">
+        <v>5033</v>
       </c>
       <c r="D1035" s="0" t="s">
-        <v>5033</v>
-      </c>
-      <c r="E1035" s="0" t="s">
         <v>5034</v>
       </c>
       <c r="F1035" s="0" t="s">
         <v>5035</v>
       </c>
-      <c r="I1035" s="0" t="s">
+      <c r="L1035" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1035" s="0" t="s">
+        <v>5035</v>
+      </c>
+    </row>
+    <row r="1036" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1036" s="0" t="s">
+        <v>5036</v>
+      </c>
+      <c r="B1036" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1036" s="0" t="s">
+        <v>5037</v>
+      </c>
+      <c r="F1036" s="0" t="s">
+        <v>5038</v>
+      </c>
+      <c r="I1036" s="0" t="s">
         <v>1039</v>
       </c>
-      <c r="L1035" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="M1035" s="0" t="s">
-        <v>5036</v>
-      </c>
-      <c r="O1035" s="0" t="s">
-        <v>5037</v>
-      </c>
-    </row>
-    <row r="1036" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1036" s="0" t="s">
-        <v>4296</v>
-      </c>
-      <c r="B1036" s="0" t="s">
-        <v>596</v>
-      </c>
-      <c r="C1036" s="0" t="s">
-        <v>5038</v>
-      </c>
-      <c r="D1036" s="0" t="s">
+      <c r="L1036" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1036" s="8" t="s">
         <v>5039</v>
       </c>
-      <c r="F1036" s="0" t="s">
+      <c r="O1036" s="5" t="s">
         <v>5040</v>
       </c>
-      <c r="L1036" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="M1036" s="0" t="s">
-        <v>5040</v>
-      </c>
-    </row>
-    <row r="1037" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="1037" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1037" s="0" t="s">
         <v>5041</v>
       </c>
@@ -41887,19 +41875,19 @@
       <c r="D1037" s="0" t="s">
         <v>5042</v>
       </c>
-      <c r="F1037" s="0" t="s">
+      <c r="I1037" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1037" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1037" s="0" t="s">
         <v>5043</v>
       </c>
-      <c r="I1037" s="0" t="s">
-        <v>1039</v>
-      </c>
-      <c r="L1037" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="M1037" s="8" t="s">
+      <c r="N1037" s="0" t="s">
         <v>5044</v>
       </c>
-      <c r="O1037" s="5" t="s">
+      <c r="O1037" s="0" t="s">
         <v>5045</v>
       </c>
     </row>
@@ -41907,198 +41895,173 @@
       <c r="A1038" s="0" t="s">
         <v>5046</v>
       </c>
-      <c r="B1038" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1038" s="0" t="s">
+      <c r="C1038" s="0" t="s">
         <v>5047</v>
       </c>
-      <c r="I1038" s="0" t="s">
-        <v>69</v>
+      <c r="H1038" s="0" t="s">
+        <v>1012</v>
       </c>
       <c r="L1038" s="0" t="s">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="M1038" s="0" t="s">
         <v>5048</v>
       </c>
-      <c r="N1038" s="0" t="s">
-        <v>5049</v>
-      </c>
-      <c r="O1038" s="0" t="s">
-        <v>5050</v>
-      </c>
     </row>
     <row r="1039" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1039" s="0" t="s">
+        <v>5049</v>
+      </c>
+      <c r="C1039" s="0" t="s">
+        <v>5050</v>
+      </c>
+      <c r="H1039" s="0" t="s">
+        <v>1394</v>
+      </c>
+      <c r="L1039" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1039" s="0" t="s">
         <v>5051</v>
-      </c>
-      <c r="C1039" s="0" t="s">
-        <v>5052</v>
-      </c>
-      <c r="H1039" s="0" t="s">
-        <v>1012</v>
-      </c>
-      <c r="L1039" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1039" s="0" t="s">
-        <v>5053</v>
       </c>
     </row>
     <row r="1040" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1040" s="0" t="s">
+        <v>5052</v>
+      </c>
+      <c r="C1040" s="0" t="s">
+        <v>5053</v>
+      </c>
+      <c r="D1040" s="0" t="s">
         <v>5054</v>
       </c>
-      <c r="C1040" s="0" t="s">
+      <c r="L1040" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1040" s="0" t="s">
         <v>5055</v>
-      </c>
-      <c r="H1040" s="0" t="s">
-        <v>1394</v>
-      </c>
-      <c r="L1040" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1040" s="0" t="s">
-        <v>5056</v>
       </c>
     </row>
     <row r="1041" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1041" s="0" t="s">
+        <v>5056</v>
+      </c>
+      <c r="C1041" s="0" t="s">
         <v>5057</v>
       </c>
-      <c r="C1041" s="0" t="s">
+      <c r="D1041" s="0" t="s">
         <v>5058</v>
       </c>
-      <c r="D1041" s="0" t="s">
+      <c r="L1041" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1041" s="0" t="s">
         <v>5059</v>
-      </c>
-      <c r="L1041" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1041" s="0" t="s">
-        <v>5060</v>
       </c>
     </row>
     <row r="1042" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1042" s="0" t="s">
+        <v>5060</v>
+      </c>
+      <c r="C1042" s="0" t="s">
         <v>5061</v>
       </c>
-      <c r="C1042" s="0" t="s">
+      <c r="E1042" s="0" t="s">
+        <v>3487</v>
+      </c>
+      <c r="L1042" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1042" s="0" t="s">
         <v>5062</v>
       </c>
-      <c r="D1042" s="0" t="s">
+    </row>
+    <row r="1043" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1043" s="0" t="s">
         <v>5063</v>
       </c>
-      <c r="L1042" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1042" s="0" t="s">
+      <c r="B1043" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1043" s="0" t="s">
+        <v>2270</v>
+      </c>
+      <c r="E1043" s="0" t="s">
         <v>5064</v>
       </c>
-    </row>
-    <row r="1043" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1043" s="0" t="s">
+      <c r="L1043" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1043" s="0" t="s">
         <v>5065</v>
       </c>
-      <c r="C1043" s="0" t="s">
+      <c r="N1043" s="5"/>
+      <c r="O1043" s="5" t="s">
         <v>5066</v>
-      </c>
-      <c r="E1043" s="0" t="s">
-        <v>3487</v>
-      </c>
-      <c r="L1043" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1043" s="0" t="s">
-        <v>5067</v>
       </c>
     </row>
     <row r="1044" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1044" s="0" t="s">
+        <v>5067</v>
+      </c>
+      <c r="B1044" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1044" s="0" t="s">
         <v>5068</v>
-      </c>
-      <c r="B1044" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1044" s="0" t="s">
-        <v>2270</v>
       </c>
       <c r="E1044" s="0" t="s">
         <v>5069</v>
       </c>
+      <c r="F1044" s="0" t="s">
+        <v>5070</v>
+      </c>
+      <c r="I1044" s="0" t="s">
+        <v>1039</v>
+      </c>
       <c r="L1044" s="0" t="s">
-        <v>107</v>
+        <v>723</v>
       </c>
       <c r="M1044" s="0" t="s">
-        <v>5070</v>
-      </c>
-      <c r="N1044" s="5"/>
+        <v>5071</v>
+      </c>
       <c r="O1044" s="5" t="s">
-        <v>5071</v>
-      </c>
-    </row>
-    <row r="1045" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5072</v>
+      </c>
+    </row>
+    <row r="1045" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1045" s="0" t="s">
-        <v>5072</v>
+        <v>5073</v>
       </c>
       <c r="B1045" s="0" t="s">
         <v>23</v>
       </c>
       <c r="D1045" s="0" t="s">
-        <v>5073</v>
+        <v>5074</v>
       </c>
       <c r="E1045" s="0" t="s">
-        <v>5074</v>
+        <v>5075</v>
       </c>
       <c r="F1045" s="0" t="s">
-        <v>5075</v>
+        <v>5076</v>
       </c>
       <c r="I1045" s="0" t="s">
         <v>1039</v>
       </c>
       <c r="L1045" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="M1045" s="0" t="s">
-        <v>5076</v>
+        <v>40</v>
+      </c>
+      <c r="M1045" s="9" t="s">
+        <v>5077</v>
+      </c>
+      <c r="N1045" s="5" t="s">
+        <v>5078</v>
       </c>
       <c r="O1045" s="5" t="s">
-        <v>5077</v>
-      </c>
-    </row>
-    <row r="1046" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1046" s="0" t="s">
-        <v>5078</v>
-      </c>
-      <c r="B1046" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1046" s="0" t="s">
         <v>5079</v>
       </c>
-      <c r="E1046" s="0" t="s">
-        <v>5080</v>
-      </c>
-      <c r="F1046" s="0" t="s">
-        <v>5081</v>
-      </c>
-      <c r="I1046" s="0" t="s">
-        <v>1039</v>
-      </c>
-      <c r="L1046" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1046" s="9" t="s">
-        <v>5082</v>
-      </c>
-      <c r="N1046" s="5" t="s">
-        <v>5083</v>
-      </c>
-      <c r="O1046" s="5" t="s">
-        <v>5084</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
@@ -42130,10 +42093,9 @@
     <hyperlink ref="N939" r:id="rId26" display="zhěnglǐ"/>
     <hyperlink ref="N940" r:id="rId27" location="Mandarin" display="shǒubì"/>
     <hyperlink ref="N941" r:id="rId28" display="rèlì"/>
-    <hyperlink ref="N953" r:id="rId29" location="Mandarin" display="zhònglì"/>
-    <hyperlink ref="N980" r:id="rId30" display="yuèjīng"/>
-    <hyperlink ref="N985" r:id="rId31" location="Mandarin" display="yǒudiǎn "/>
-    <hyperlink ref="N1046" r:id="rId32" display="chuàngxīn"/>
+    <hyperlink ref="N979" r:id="rId29" display="yuèjīng"/>
+    <hyperlink ref="N984" r:id="rId30" location="Mandarin" display="yǒudiǎn "/>
+    <hyperlink ref="N1045" r:id="rId31" display="chuàngxīn"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -42143,7 +42105,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId33"/>
+    <tablePart r:id="rId32"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bug fix in flashcards
yes I am stupid. be nice
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -313,7 +313,7 @@
     <t xml:space="preserve">agreeable/harmonic/fitting</t>
   </si>
   <si>
-    <t xml:space="preserve">harmonically</t>
+    <t xml:space="preserve">harmonically/agreeably</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -5792,7 +5792,7 @@
     <t xml:space="preserve">meir</t>
   </si>
   <si>
-    <t xml:space="preserve">charisma</t>
+    <t xml:space="preserve">charisma/charm</t>
   </si>
   <si>
     <t xml:space="preserve">charm/convince/assure/sweet talk/persuade</t>
@@ -7431,7 +7431,7 @@
     <t xml:space="preserve">niy</t>
   </si>
   <si>
-    <t xml:space="preserve">learning/analysis/research</t>
+    <t xml:space="preserve">learning/analysis/research/lesson</t>
   </si>
   <si>
     <t xml:space="preserve">learn/study/practice/analyze/investigate</t>
@@ -15824,13 +15824,13 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A958" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B958" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A958" activeCellId="0" sqref="A958"/>
-      <selection pane="topRight" activeCell="F978" activeCellId="0" sqref="F978"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.5"/>

</xml_diff>

<commit_message>
dict updates and color variables
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7731" uniqueCount="5051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7732" uniqueCount="5051">
   <si>
     <t xml:space="preserve">Orostara</t>
   </si>
@@ -166,10 +166,10 @@
     <t xml:space="preserve">front</t>
   </si>
   <si>
-    <t xml:space="preserve">forwards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(physically) in front of/next/beyond/(temporally) before</t>
+    <t xml:space="preserve">forwards/forward/ahead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(physically) in front of/next/beyond/ahead of/(temporally) before</t>
   </si>
   <si>
     <t xml:space="preserve">direction/preposition</t>
@@ -1916,7 +1916,7 @@
     <t xml:space="preserve">used as a slur of sorts to talk about people who Venusians (mostly) feel aren't pulling their weight and are a waste of resources</t>
   </si>
   <si>
-    <t xml:space="preserve">parasite/(colloquially) leech</t>
+    <t xml:space="preserve">expense/(colloquially) leech/parasite</t>
   </si>
   <si>
     <t xml:space="preserve">spend/expend/use up/waste/consume</t>
@@ -2189,7 +2189,7 @@
     <t xml:space="preserve">eat</t>
   </si>
   <si>
-    <t xml:space="preserve">edible</t>
+    <t xml:space="preserve">edible/hungry</t>
   </si>
   <si>
     <t xml:space="preserve">吃</t>
@@ -6947,7 +6947,7 @@
     <t xml:space="preserve">need/depend/rely on/require</t>
   </si>
   <si>
-    <t xml:space="preserve">necessary/essential</t>
+    <t xml:space="preserve">necessary/essential/needed</t>
   </si>
   <si>
     <t xml:space="preserve">necessarily</t>
@@ -8409,7 +8409,7 @@
     <t xml:space="preserve">back</t>
   </si>
   <si>
-    <t xml:space="preserve">backwards</t>
+    <t xml:space="preserve">backwards/backward</t>
   </si>
   <si>
     <t xml:space="preserve">(physically) behind/in back of/last/(temporally) after/next</t>
@@ -8823,7 +8823,7 @@
     <t xml:space="preserve">pet</t>
   </si>
   <si>
-    <t xml:space="preserve">seat/(colloquially) butt</t>
+    <t xml:space="preserve">seat/chair/(colloquially) butt</t>
   </si>
   <si>
     <t xml:space="preserve">sit</t>
@@ -9375,7 +9375,7 @@
     <t xml:space="preserve">animalistic</t>
   </si>
   <si>
-    <t xml:space="preserve">animalisticly</t>
+    <t xml:space="preserve">animalistically</t>
   </si>
   <si>
     <t xml:space="preserve">পশু</t>
@@ -11682,7 +11682,7 @@
     <t xml:space="preserve">repeat/copy/duplicate</t>
   </si>
   <si>
-    <t xml:space="preserve">repetitive</t>
+    <t xml:space="preserve">repetitive/repeated</t>
   </si>
   <si>
     <t xml:space="preserve">repetitively/again</t>
@@ -15824,13 +15824,13 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A116" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B116" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
+      <selection pane="topRight" activeCell="G139" activeCellId="0" sqref="G139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.5"/>
@@ -31607,6 +31607,9 @@
       </c>
       <c r="B632" s="0" t="s">
         <v>23</v>
+      </c>
+      <c r="D632" s="0" t="s">
+        <v>3102</v>
       </c>
       <c r="E632" s="0" t="s">
         <v>3102</v>

</xml_diff>

<commit_message>
separated everything into real pages
and added some stuff: home page, socials page, rhyming dict, etc
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -15965,11 +15965,11 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A489" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E510" activeCellId="0" sqref="E510"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1018" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1053" activeCellId="0" sqref="J1053"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.71875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.5"/>

</xml_diff>

<commit_message>
alternate spellings supported now!
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -391,7 +391,7 @@
     <t xml:space="preserve">akmin/akimin</t>
   </si>
   <si>
-    <t xml:space="preserve">for discrete times; 'ten minutes ago'; see 'xamin' for general times like 'in the last few minutes'</t>
+    <t xml:space="preserve">for discrete times; 'ten minutes ago'; see 'rimin' for general times like 'in the last few minutes'</t>
   </si>
   <si>
     <t xml:space="preserve">last minute </t>
@@ -430,7 +430,7 @@
     <t xml:space="preserve">akmon/akimon</t>
   </si>
   <si>
-    <t xml:space="preserve">for discrete times; 'ten months ago'; see 'xamon' for general times like 'in the last few months'</t>
+    <t xml:space="preserve">for discrete times; 'ten months ago'; see 'rimon' for general times like 'in the last few months'</t>
   </si>
   <si>
     <t xml:space="preserve">last month</t>
@@ -946,7 +946,7 @@
     <t xml:space="preserve">aksek/akisek</t>
   </si>
   <si>
-    <t xml:space="preserve">for discrete times; 'ten seconds ago'; see 'xasek' for general times like 'in the last few seconds'</t>
+    <t xml:space="preserve">for discrete times; 'ten seconds ago'; see 'risek' for general times like 'in the last few seconds'</t>
   </si>
   <si>
     <t xml:space="preserve">last second</t>
@@ -961,7 +961,7 @@
     <t xml:space="preserve">aksem/akisem</t>
   </si>
   <si>
-    <t xml:space="preserve">for discrete times; 'ten weeks ago'; see 'xasem' for general times like 'in the last few weeks'</t>
+    <t xml:space="preserve">for discrete times; 'ten weeks ago'; see 'risem' for general times like 'in the last few weeks'</t>
   </si>
   <si>
     <t xml:space="preserve">next week</t>
@@ -1063,7 +1063,7 @@
     <t xml:space="preserve">akten/akiten</t>
   </si>
   <si>
-    <t xml:space="preserve">for discrete times; 'ten days ago'; see 'xaten' for general times like 'in the last few days'</t>
+    <t xml:space="preserve">for discrete times; 'ten days ago'; see 'riten' for general times like 'in the last few days'</t>
   </si>
   <si>
     <t xml:space="preserve">yesterday/last day</t>
@@ -1165,7 +1165,7 @@
     <t xml:space="preserve">akxas/akixas</t>
   </si>
   <si>
-    <t xml:space="preserve">for discrete times; 'ten hours ago'; see 'xaxas' for general times like 'in the last few hours'</t>
+    <t xml:space="preserve">for discrete times; 'ten hours ago'; see 'rixas' for general times like 'in the last few hours'</t>
   </si>
   <si>
     <t xml:space="preserve">last hour</t>
@@ -16104,11 +16104,11 @@
   </sheetPr>
   <dimension ref="A1:Q1049"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1017" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1051" activeCellId="0" sqref="B1051"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.73828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.5"/>

</xml_diff>